<commit_message>
Thêm tính năng kiểm tra thiết bị mới cắm vào
</commit_message>
<xml_diff>
--- a/Functions.xlsx
+++ b/Functions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VNPT\Tinh uy\Quan tri mang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E0FDF0A-6690-4183-8B95-2C66302B47EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9D809D9-399F-4F74-B8CE-4A29C14A441A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
-  <si>
-    <t>DANH SÁCH TÍNH NĂNG</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="13">
   <si>
     <t>Tính năng</t>
   </si>
@@ -52,13 +49,29 @@
   </si>
   <si>
     <t>Kiểm tra port</t>
+  </si>
+  <si>
+    <t>Kiểm tra thay đổi config</t>
+  </si>
+  <si>
+    <t>Cảnh báo khi có thiết bị lạ cắm vào</t>
+  </si>
+  <si>
+    <t>Tất cả các tính năng đều thông báo thông qua Telegram bot</t>
+  </si>
+  <si>
+    <t>DANH SÁCH TÍNH NĂNG PHẦN MỀM
+QUẢN TRỊ MẠNG</t>
+  </si>
+  <si>
+    <t>Thực thi lệnh thông qua Telegram</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,12 +95,24 @@
     <font>
       <b/>
       <sz val="12"/>
-      <color theme="1"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="9" tint="-0.499984740745262"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -100,8 +125,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -109,25 +140,131 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -411,142 +548,166 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.28515625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-    </row>
-    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="13"/>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="B4" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="14"/>
+      <c r="E4" s="15"/>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="B5" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="14"/>
+      <c r="E5" s="15"/>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="B6" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="14"/>
+      <c r="E6" s="15"/>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="14"/>
+      <c r="E7" s="15"/>
     </row>
     <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
+      <c r="A8" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="15"/>
     </row>
     <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
+      <c r="A9" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="14"/>
+      <c r="E9" s="15"/>
     </row>
     <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+      <c r="A10" s="8"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="15"/>
     </row>
     <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
+      <c r="A11" s="8"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="17"/>
     </row>
     <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
+      <c r="A12" s="1"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
+      <c r="A13" s="1"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
+      <c r="A14" s="1"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="A1:E1"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>